<commit_message>
#362 Drafted Multi timezone applications.
</commit_message>
<xml_diff>
--- a/Articles/362/model/SupportPlanning/data/wb.xlsx
+++ b/Articles/362/model/SupportPlanning/data/wb.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\u\s\How To\feature-branch-362-ref-timezone\Articles\362\model\SupportPlanning\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85AC179-1DE2-416B-9525-0C6C6ECF9689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-24735" yWindow="-2160" windowWidth="16125" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d\.m\.yy\ hh:mm"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +58,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +340,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C3:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>